<commit_message>
Finished tasks for chapter 3
</commit_message>
<xml_diff>
--- a/Tutorial 2/Chapter 3/Scatter.xlsx
+++ b/Tutorial 2/Chapter 3/Scatter.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howde\Documents\Repos\MGMT220\Tutorial 2\Chapter 3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC84905D-1407-4BFB-98B2-794005D19EFE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="165" windowWidth="9720" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="5768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -153,8 +159,1054 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Observations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-37</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-33</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-29</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-14CE-49A1-B2E5-83DD071FFED2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="398547568"/>
+        <c:axId val="398545968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="398547568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398545968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="398545968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="398547568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>402431</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>50005</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>88106</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>59530</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73EB3F58-3B88-44A5-B26F-F93BA4D67A97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -200,7 +1252,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,9 +1285,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,6 +1337,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -443,17 +1529,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="15.4"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="12.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1328125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -695,5 +1783,6 @@
     <oddHeader>&amp;A</oddHeader>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>